<commit_message>
fixes database names for biosphere3 exchanges
</commit_message>
<xml_diff>
--- a/inv_import_V1.xlsx
+++ b/inv_import_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5A6C1-EEEF-4A06-BE84-E61A150E4884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA9BDB1-6316-470A-8941-AB5793A0048A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="5460" windowWidth="15630" windowHeight="11835" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="830" yWindow="-110" windowWidth="18480" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Delete Exchanges" sheetId="3" r:id="rId3"/>
     <sheet name="Add Exchanges" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Add Exchanges'!$A$1:$L$93</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="303">
   <si>
     <t>US</t>
   </si>
@@ -1442,7 +1445,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1452,7 +1455,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1808,29 +1813,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB01F63A-80EB-45BB-BC08-862364DEF79F}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.453125" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="225.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="225.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>283</v>
       </c>
@@ -1858,14 +1863,14 @@
       <c r="I1" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>290</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>50</v>
       </c>
@@ -1890,14 +1895,14 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="10">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>50</v>
       </c>
@@ -1922,14 +1927,14 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="10">
         <v>2</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>50</v>
       </c>
@@ -1954,14 +1959,14 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="10">
         <v>3</v>
       </c>
       <c r="K4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -1986,11 +1991,11 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>50</v>
       </c>
@@ -2015,14 +2020,14 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="10">
         <v>5</v>
       </c>
       <c r="K6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>50</v>
       </c>
@@ -2047,11 +2052,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -2076,11 +2081,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>50</v>
       </c>
@@ -2105,11 +2110,11 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>50</v>
       </c>
@@ -2134,11 +2139,11 @@
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -2163,11 +2168,11 @@
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -2192,11 +2197,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="10">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
@@ -2221,14 +2226,14 @@
       <c r="I13" s="7">
         <v>1</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="11">
         <v>12</v>
       </c>
       <c r="K13" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -2253,11 +2258,11 @@
       <c r="I14">
         <v>1</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="10">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>50</v>
       </c>
@@ -2282,11 +2287,11 @@
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="10">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -2311,11 +2316,11 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="10">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>55</v>
       </c>
@@ -2340,11 +2345,11 @@
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="10">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -2369,11 +2374,11 @@
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="10">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2398,11 +2403,11 @@
       <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>50</v>
       </c>
@@ -2427,14 +2432,14 @@
       <c r="I20">
         <v>1</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="10">
         <v>19</v>
       </c>
       <c r="K20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -2459,14 +2464,14 @@
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="10">
         <v>20</v>
       </c>
       <c r="K21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -2491,14 +2496,14 @@
       <c r="I22">
         <v>1</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="10">
         <v>21</v>
       </c>
       <c r="K22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -2523,11 +2528,11 @@
       <c r="I23">
         <v>1</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="10">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="7" t="s">
         <v>55</v>
       </c>
@@ -2552,11 +2557,11 @@
       <c r="I24" s="7">
         <v>1</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="11">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -2581,11 +2586,11 @@
       <c r="I25">
         <v>1</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="10">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -2610,11 +2615,11 @@
       <c r="I26">
         <v>1</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="10">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>50</v>
       </c>
@@ -2639,11 +2644,11 @@
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -2668,11 +2673,11 @@
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="10">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>50</v>
       </c>
@@ -2697,14 +2702,14 @@
       <c r="I29">
         <v>1</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="10">
         <v>28</v>
       </c>
       <c r="K29" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" s="7" t="s">
         <v>50</v>
       </c>
@@ -2729,14 +2734,14 @@
       <c r="I30" s="7">
         <v>1</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="11">
         <v>29</v>
       </c>
       <c r="K30" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>50</v>
       </c>
@@ -2761,11 +2766,11 @@
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>50</v>
       </c>
@@ -2787,11 +2792,11 @@
       <c r="I32">
         <v>1</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="10">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -2813,11 +2818,11 @@
       <c r="I33">
         <v>1</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J33" s="10">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>55</v>
       </c>
@@ -2839,11 +2844,11 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="J34" s="5">
+      <c r="J34" s="10">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>55</v>
       </c>
@@ -2865,11 +2870,11 @@
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J35" s="10">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -2891,14 +2896,14 @@
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="J36" s="5">
+      <c r="J36" s="10">
         <v>35</v>
       </c>
       <c r="K36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -2920,15 +2925,12 @@
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J37" s="10">
         <v>36</v>
       </c>
       <c r="K37" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J38" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -2942,20 +2944,20 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>293</v>
       </c>
@@ -2971,7 +2973,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2985,7 +2987,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -2999,7 +3001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3013,7 +3015,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -3051,22 +3053,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>283</v>
       </c>
@@ -3099,7 +3101,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>47</v>
       </c>
@@ -3119,7 +3121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -3139,7 +3141,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="str">
         <f>'Copy Activities'!B3</f>
         <v>gravel and sand quarry operation</v>
@@ -3158,7 +3160,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="str">
         <f t="shared" ref="B5:B13" si="0">B4</f>
         <v>gravel and sand quarry operation</v>
@@ -3178,7 +3180,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3198,7 +3200,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3218,7 +3220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3238,7 +3240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3258,7 +3260,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3278,7 +3280,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3298,7 +3300,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3318,7 +3320,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>gravel and sand quarry operation</v>
@@ -3338,7 +3340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3361,7 +3363,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B15" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3384,7 +3386,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3407,7 +3409,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3430,7 +3432,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3453,7 +3455,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3476,7 +3478,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3499,7 +3501,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3522,7 +3524,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3545,7 +3547,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3568,7 +3570,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3591,7 +3593,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3614,7 +3616,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3637,7 +3639,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3660,7 +3662,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3683,7 +3685,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3706,7 +3708,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3729,7 +3731,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3752,7 +3754,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3775,7 +3777,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3798,7 +3800,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3821,7 +3823,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3844,7 +3846,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3867,7 +3869,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3890,7 +3892,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3913,7 +3915,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3936,7 +3938,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3959,7 +3961,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -3982,7 +3984,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4005,7 +4007,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4028,7 +4030,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4051,7 +4053,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4074,7 +4076,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4097,7 +4099,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4120,7 +4122,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B48" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4143,7 +4145,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4166,7 +4168,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4189,7 +4191,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4212,7 +4214,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4235,7 +4237,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4258,7 +4260,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4281,7 +4283,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4304,7 +4306,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4327,7 +4329,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4350,7 +4352,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4373,7 +4375,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4396,7 +4398,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4419,7 +4421,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4442,7 +4444,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4465,7 +4467,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4488,7 +4490,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4511,7 +4513,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4534,7 +4536,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4557,7 +4559,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4580,7 +4582,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4603,7 +4605,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4626,7 +4628,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" t="str">
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
@@ -4649,7 +4651,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" t="str">
         <f>'Copy Activities'!$B$5</f>
         <v>transformer production, high voltage use</v>
@@ -4668,7 +4670,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B72" t="str">
         <f>'Copy Activities'!$B$5</f>
         <v>transformer production, high voltage use</v>
@@ -4687,7 +4689,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B73" t="str">
         <f>'Copy Activities'!$B$5</f>
         <v>transformer production, high voltage use</v>
@@ -4706,7 +4708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B74" t="str">
         <f>'Copy Activities'!B6</f>
         <v>tap water production, underground water without treatment</v>
@@ -4738,34 +4740,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>283</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>294</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -4777,7 +4779,7 @@
       <c r="F1" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>297</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -4799,7 +4801,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -4807,7 +4809,7 @@
         <f>'Create Activities'!C2</f>
         <v>embankment earthfill</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="10">
         <f>'Create Activities'!J2</f>
         <v>1</v>
       </c>
@@ -4820,7 +4822,7 @@
       <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H2" s="4">
@@ -4836,7 +4838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4844,7 +4846,7 @@
         <f>'Create Activities'!C34</f>
         <v>soil organic carbon</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="10">
         <f>'Create Activities'!J34</f>
         <v>33</v>
       </c>
@@ -4857,7 +4859,7 @@
       <c r="F3" t="s">
         <v>57</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H3">
@@ -4873,7 +4875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4881,7 +4883,7 @@
         <f>'Create Activities'!C34</f>
         <v>soil organic carbon</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="10">
         <f>'Create Activities'!J34</f>
         <v>33</v>
       </c>
@@ -4894,7 +4896,7 @@
       <c r="F4" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>67</v>
       </c>
       <c r="H4" s="3">
@@ -4910,7 +4912,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -4918,7 +4920,7 @@
         <f>'Create Activities'!C34</f>
         <v>soil organic carbon</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="10">
         <f>'Create Activities'!J34</f>
         <v>33</v>
       </c>
@@ -4931,7 +4933,7 @@
       <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="H5" s="3">
@@ -4947,7 +4949,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4955,7 +4957,7 @@
         <f>'Create Activities'!C34</f>
         <v>soil organic carbon</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="10">
         <f>'Create Activities'!J34</f>
         <v>33</v>
       </c>
@@ -4968,7 +4970,7 @@
       <c r="F6" t="s">
         <v>65</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>66</v>
       </c>
       <c r="H6">
@@ -4984,7 +4986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" ref="A7:E7" si="0">A2</f>
         <v>nrel psh</v>
@@ -4993,7 +4995,7 @@
         <f t="shared" si="0"/>
         <v>embankment earthfill</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -5008,7 +5010,7 @@
         <f>B6</f>
         <v>soil organic carbon</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="10">
         <f>C6</f>
         <v>33</v>
       </c>
@@ -5025,7 +5027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -5033,7 +5035,7 @@
         <f>'Create Activities'!C35</f>
         <v>sand in soil</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="10">
         <f>'Create Activities'!J35</f>
         <v>34</v>
       </c>
@@ -5041,12 +5043,12 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H8">
@@ -5062,7 +5064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" ref="A9:E11" si="1">A8</f>
         <v>nrel psh</v>
@@ -5071,7 +5073,7 @@
         <f t="shared" si="1"/>
         <v>sand in soil</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="10">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -5080,13 +5082,13 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>nrel psh</v>
+        <v>biosphere3</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ref="F9:K11" si="2">F4</f>
         <v>Transformation, to unspecified</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9" s="10" t="str">
         <f t="shared" si="2"/>
         <v>512a5356-8059-4772-a43f-42e3c4f3d299</v>
       </c>
@@ -5107,7 +5109,7 @@
         <v>biosphere</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="1"/>
         <v>nrel psh</v>
@@ -5116,7 +5118,7 @@
         <f t="shared" si="1"/>
         <v>sand in soil</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="10">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -5125,13 +5127,13 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>nrel psh</v>
+        <v>biosphere3</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
         <v>Transformation, from unspecified</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" s="10" t="str">
         <f t="shared" si="2"/>
         <v>512a5356-8059-4772-a43f-42e3c4f3d299</v>
       </c>
@@ -5152,7 +5154,7 @@
         <v>biosphere</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
         <v>nrel psh</v>
@@ -5161,7 +5163,7 @@
         <f t="shared" si="1"/>
         <v>sand in soil</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="10">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -5170,13 +5172,13 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>nrel psh</v>
+        <v>biosphere3</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
         <v>Occupation, mineral extraction site</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11" s="10" t="str">
         <f t="shared" si="2"/>
         <v>379ba5c9-5c3a-43d0-8e2d-605ad9c39e46</v>
       </c>
@@ -5197,7 +5199,7 @@
         <v>biosphere</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" ref="A12:K12" si="3">A7</f>
         <v>nrel psh</v>
@@ -5206,7 +5208,7 @@
         <f t="shared" si="3"/>
         <v>embankment earthfill</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -5221,7 +5223,7 @@
         <f>B11</f>
         <v>sand in soil</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="10">
         <f>C11</f>
         <v>34</v>
       </c>
@@ -5240,7 +5242,7 @@
         <v>technosphere</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -5248,7 +5250,7 @@
         <f>'Delete Exchanges'!B4</f>
         <v>gravel and sand quarry operation</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="10" t="str">
         <f>'Delete Exchanges'!C4</f>
         <v>14ad7fee91d429fc020451a3e5c65feb</v>
       </c>
@@ -5262,7 +5264,7 @@
         <f>'Create Activities'!C20</f>
         <v>electricity, construction</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="10">
         <f>'Create Activities'!J20</f>
         <v>19</v>
       </c>
@@ -5279,7 +5281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -5287,7 +5289,7 @@
         <f>'Create Activities'!C3</f>
         <v>embankment rockfill</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="10">
         <f>'Create Activities'!J3</f>
         <v>2</v>
       </c>
@@ -5302,7 +5304,7 @@
         <f>B13</f>
         <v>gravel and sand quarry operation</v>
       </c>
-      <c r="G14" t="str">
+      <c r="G14" s="10" t="str">
         <f>C13</f>
         <v>14ad7fee91d429fc020451a3e5c65feb</v>
       </c>
@@ -5319,7 +5321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -5327,7 +5329,7 @@
         <f>'Create Activities'!C36</f>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="10">
         <f>'Create Activities'!J36</f>
         <v>35</v>
       </c>
@@ -5340,7 +5342,7 @@
       <c r="F15" t="s">
         <v>86</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="10" t="s">
         <v>97</v>
       </c>
       <c r="H15" s="3">
@@ -5356,7 +5358,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" ref="A16:A41" si="4">A15</f>
         <v>nrel psh</v>
@@ -5365,7 +5367,7 @@
         <f t="shared" ref="B16:B41" si="5">B15</f>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="10">
         <f t="shared" ref="C16:C41" si="6">C15</f>
         <v>35</v>
       </c>
@@ -5379,7 +5381,7 @@
       <c r="F16" t="s">
         <v>29</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="10" t="s">
         <v>98</v>
       </c>
       <c r="H16" s="3">
@@ -5395,7 +5397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5404,7 +5406,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5418,7 +5420,7 @@
       <c r="F17" t="s">
         <v>87</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="10" t="s">
         <v>99</v>
       </c>
       <c r="H17" s="3">
@@ -5434,7 +5436,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5443,7 +5445,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5457,7 +5459,7 @@
       <c r="F18" t="s">
         <v>88</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="10" t="s">
         <v>100</v>
       </c>
       <c r="H18" s="3">
@@ -5473,7 +5475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5482,7 +5484,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5496,7 +5498,7 @@
       <c r="F19" t="s">
         <v>89</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="10" t="s">
         <v>101</v>
       </c>
       <c r="H19" s="3">
@@ -5512,7 +5514,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5521,7 +5523,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5535,7 +5537,7 @@
       <c r="F20" t="s">
         <v>90</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="10" t="s">
         <v>102</v>
       </c>
       <c r="H20" s="3">
@@ -5551,7 +5553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5560,7 +5562,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5574,7 +5576,7 @@
       <c r="F21" t="s">
         <v>91</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="10" t="s">
         <v>103</v>
       </c>
       <c r="H21" s="3">
@@ -5590,7 +5592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5599,7 +5601,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5613,7 +5615,7 @@
       <c r="F22" t="s">
         <v>92</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="10" t="s">
         <v>104</v>
       </c>
       <c r="H22" s="3">
@@ -5629,7 +5631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5638,7 +5640,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5652,7 +5654,7 @@
       <c r="F23" t="s">
         <v>92</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="10" t="s">
         <v>105</v>
       </c>
       <c r="H23" s="3">
@@ -5668,7 +5670,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5677,7 +5679,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5691,7 +5693,7 @@
       <c r="F24" t="s">
         <v>92</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="10" t="s">
         <v>106</v>
       </c>
       <c r="H24" s="3">
@@ -5707,7 +5709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5716,7 +5718,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5730,7 +5732,7 @@
       <c r="F25" t="s">
         <v>92</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="10" t="s">
         <v>107</v>
       </c>
       <c r="H25">
@@ -5746,7 +5748,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5755,7 +5757,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5769,7 +5771,7 @@
       <c r="F26" t="s">
         <v>92</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="10" t="s">
         <v>108</v>
       </c>
       <c r="H26">
@@ -5785,7 +5787,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5794,7 +5796,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5808,7 +5810,7 @@
       <c r="F27" t="s">
         <v>92</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="10" t="s">
         <v>109</v>
       </c>
       <c r="H27" s="3">
@@ -5824,7 +5826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5833,7 +5835,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5847,7 +5849,7 @@
       <c r="F28" t="s">
         <v>92</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="10" t="s">
         <v>110</v>
       </c>
       <c r="H28" s="3">
@@ -5863,7 +5865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5872,7 +5874,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5886,7 +5888,7 @@
       <c r="F29" t="s">
         <v>92</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H29">
@@ -5902,7 +5904,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5911,7 +5913,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5925,7 +5927,7 @@
       <c r="F30" t="s">
         <v>93</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="10" t="s">
         <v>112</v>
       </c>
       <c r="H30" s="3">
@@ -5941,7 +5943,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5950,7 +5952,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -5964,7 +5966,7 @@
       <c r="F31" t="s">
         <v>93</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H31" s="3">
@@ -5980,7 +5982,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -5989,7 +5991,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6003,7 +6005,7 @@
       <c r="F32" t="s">
         <v>93</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="H32" s="3">
@@ -6019,7 +6021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6028,7 +6030,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6042,7 +6044,7 @@
       <c r="F33" t="s">
         <v>93</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="10" t="s">
         <v>115</v>
       </c>
       <c r="H33" s="3">
@@ -6058,7 +6060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6067,7 +6069,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6081,7 +6083,7 @@
       <c r="F34" t="s">
         <v>93</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H34" s="3">
@@ -6097,7 +6099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6106,7 +6108,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6120,7 +6122,7 @@
       <c r="F35" t="s">
         <v>94</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="10" t="s">
         <v>117</v>
       </c>
       <c r="H35" s="3">
@@ -6136,7 +6138,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6145,7 +6147,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6159,7 +6161,7 @@
       <c r="F36" t="s">
         <v>94</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="10" t="s">
         <v>117</v>
       </c>
       <c r="H36" s="3">
@@ -6175,7 +6177,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6184,7 +6186,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6198,7 +6200,7 @@
       <c r="F37" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="10" t="s">
         <v>118</v>
       </c>
       <c r="H37" s="3">
@@ -6214,7 +6216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6223,7 +6225,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6237,7 +6239,7 @@
       <c r="F38" t="s">
         <v>94</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="10" t="s">
         <v>118</v>
       </c>
       <c r="H38" s="3">
@@ -6253,7 +6255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6262,7 +6264,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6276,7 +6278,7 @@
       <c r="F39" t="s">
         <v>95</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="10" t="s">
         <v>119</v>
       </c>
       <c r="H39" s="3">
@@ -6292,7 +6294,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6301,7 +6303,7 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
@@ -6315,7 +6317,7 @@
       <c r="F40" t="s">
         <v>95</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="10" t="s">
         <v>120</v>
       </c>
       <c r="H40">
@@ -6331,7 +6333,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f t="shared" si="4"/>
         <v>nrel psh</v>
@@ -6340,21 +6342,20 @@
         <f t="shared" si="5"/>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="10">
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E41" t="str">
-        <f t="shared" si="7"/>
-        <v>ecoinvent3.8 cut-off</v>
+      <c r="E41" t="s">
+        <v>46</v>
       </c>
       <c r="F41" t="s">
         <v>96</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="10" t="s">
         <v>121</v>
       </c>
       <c r="H41">
@@ -6370,7 +6371,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -6378,7 +6379,7 @@
         <f>B12</f>
         <v>embankment earthfill</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="10">
         <f>C12</f>
         <v>1</v>
       </c>
@@ -6393,7 +6394,7 @@
         <f>B41</f>
         <v>embankement earthfill operation</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="10">
         <f>C41</f>
         <v>35</v>
       </c>
@@ -6410,7 +6411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -6418,7 +6419,7 @@
         <f>'Create Activities'!C4</f>
         <v>rip rap slope protection</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="10">
         <f>'Create Activities'!J4</f>
         <v>3</v>
       </c>
@@ -6432,7 +6433,7 @@
         <f>'Create Activities'!C3</f>
         <v>embankment rockfill</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="10">
         <f>'Create Activities'!J3</f>
         <v>2</v>
       </c>
@@ -6449,7 +6450,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -6457,7 +6458,7 @@
         <f>'Create Activities'!C33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="10">
         <f>'Create Activities'!J33</f>
         <v>32</v>
       </c>
@@ -6470,7 +6471,7 @@
       <c r="F44" t="s">
         <v>142</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="10" t="s">
         <v>141</v>
       </c>
       <c r="H44">
@@ -6486,7 +6487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>A44</f>
         <v>nrel psh</v>
@@ -6495,7 +6496,7 @@
         <f>B44</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="10">
         <f>C44</f>
         <v>32</v>
       </c>
@@ -6508,7 +6509,7 @@
       <c r="F45" t="s">
         <v>4</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="10" t="s">
         <v>143</v>
       </c>
       <c r="H45">
@@ -6524,7 +6525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>A45</f>
         <v>nrel psh</v>
@@ -6533,7 +6534,7 @@
         <f t="shared" ref="B46:E47" si="8">B45</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="10">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
@@ -6547,7 +6548,7 @@
       <c r="F46" t="s">
         <v>144</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="10" t="s">
         <v>145</v>
       </c>
       <c r="H46">
@@ -6563,7 +6564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>A46</f>
         <v>nrel psh</v>
@@ -6572,7 +6573,7 @@
         <f t="shared" si="8"/>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="10">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
@@ -6585,7 +6586,7 @@
       <c r="F47" t="s">
         <v>146</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="10" t="s">
         <v>147</v>
       </c>
       <c r="H47">
@@ -6601,7 +6602,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>A47</f>
         <v>nrel psh</v>
@@ -6610,7 +6611,7 @@
         <f>B47</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="10">
         <f>C47</f>
         <v>32</v>
       </c>
@@ -6623,7 +6624,7 @@
       <c r="F48" t="s">
         <v>148</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="10" t="s">
         <v>149</v>
       </c>
       <c r="H48">
@@ -6639,7 +6640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>A48</f>
         <v>nrel psh</v>
@@ -6648,7 +6649,7 @@
         <f>B48</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="10">
         <f>C48</f>
         <v>32</v>
       </c>
@@ -6661,7 +6662,7 @@
       <c r="F49" t="s">
         <v>72</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="10" t="s">
         <v>73</v>
       </c>
       <c r="H49">
@@ -6677,7 +6678,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -6685,7 +6686,7 @@
         <f>'Create Activities'!C33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="10">
         <f>C49</f>
         <v>32</v>
       </c>
@@ -6698,7 +6699,7 @@
       <c r="F50" t="s">
         <v>79</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="10" t="s">
         <v>150</v>
       </c>
       <c r="H50">
@@ -6714,7 +6715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -6722,7 +6723,7 @@
         <f>B50</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="10">
         <f>C50</f>
         <v>32</v>
       </c>
@@ -6735,7 +6736,7 @@
       <c r="F51" t="s">
         <v>152</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="10" t="s">
         <v>153</v>
       </c>
       <c r="H51">
@@ -6751,7 +6752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -6759,7 +6760,7 @@
         <f>B51</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="10">
         <f>C51</f>
         <v>32</v>
       </c>
@@ -6772,7 +6773,7 @@
       <c r="F52" t="s">
         <v>154</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="10" t="s">
         <v>155</v>
       </c>
       <c r="H52">
@@ -6788,7 +6789,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>'Copy Activities'!$D$4</f>
         <v>nrel psh</v>
@@ -6797,7 +6798,7 @@
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
       </c>
-      <c r="C53" s="5" t="str">
+      <c r="C53" s="10" t="str">
         <f>'Copy Activities'!$C$4</f>
         <v>1772b4b7346b1b9acb7d0b572a9e75bf</v>
       </c>
@@ -6810,7 +6811,7 @@
       <c r="F53" t="s">
         <v>159</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="10" t="s">
         <v>217</v>
       </c>
       <c r="H53">
@@ -6826,7 +6827,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>'Copy Activities'!$D$4</f>
         <v>nrel psh</v>
@@ -6835,7 +6836,7 @@
         <f>'Copy Activities'!$B$4</f>
         <v>market for diesel, low-sulfur</v>
       </c>
-      <c r="C54" s="5" t="str">
+      <c r="C54" s="10" t="str">
         <f>'Copy Activities'!$C$4</f>
         <v>1772b4b7346b1b9acb7d0b572a9e75bf</v>
       </c>
@@ -6848,7 +6849,7 @@
       <c r="F54" t="s">
         <v>146</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="10" t="s">
         <v>147</v>
       </c>
       <c r="H54">
@@ -6864,7 +6865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>45</v>
       </c>
@@ -6872,7 +6873,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -6887,7 +6888,7 @@
         <f>'Copy Activities'!B4</f>
         <v>market for diesel, low-sulfur</v>
       </c>
-      <c r="G55" t="str">
+      <c r="G55" s="10" t="str">
         <f>'Copy Activities'!C4</f>
         <v>1772b4b7346b1b9acb7d0b572a9e75bf</v>
       </c>
@@ -6904,7 +6905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -6912,7 +6913,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -6925,7 +6926,7 @@
       <c r="F56" t="s">
         <v>219</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="10" t="s">
         <v>218</v>
       </c>
       <c r="H56">
@@ -6941,7 +6942,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -6949,7 +6950,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -6962,7 +6963,7 @@
       <c r="F57" t="s">
         <v>146</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="10" t="s">
         <v>147</v>
       </c>
       <c r="H57">
@@ -6978,7 +6979,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -6986,7 +6987,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -6999,7 +7000,7 @@
       <c r="F58" t="s">
         <v>220</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="10" t="s">
         <v>221</v>
       </c>
       <c r="H58">
@@ -7015,7 +7016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -7023,7 +7024,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7036,7 +7037,7 @@
       <c r="F59" t="s">
         <v>222</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="10" t="s">
         <v>223</v>
       </c>
       <c r="H59">
@@ -7052,7 +7053,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>45</v>
       </c>
@@ -7060,7 +7061,7 @@
         <f>'Create Activities'!C5</f>
         <v>concrete, dam face materials</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="10">
         <f>'Create Activities'!J5</f>
         <v>4</v>
       </c>
@@ -7074,7 +7075,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7091,7 +7092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -7099,7 +7100,7 @@
         <f>'Create Activities'!C6</f>
         <v>concrete, tunnel lining</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="10">
         <f>'Create Activities'!J6</f>
         <v>5</v>
       </c>
@@ -7113,7 +7114,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="G61" s="5">
+      <c r="G61" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7130,7 +7131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -7138,7 +7139,7 @@
         <f>'Create Activities'!C7</f>
         <v>concrete, powerhouse</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="10">
         <f>'Create Activities'!J7</f>
         <v>6</v>
       </c>
@@ -7152,7 +7153,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7169,7 +7170,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>45</v>
       </c>
@@ -7177,7 +7178,7 @@
         <f>'Create Activities'!C8</f>
         <v>concrete, RCC dam type</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="10">
         <f>'Create Activities'!J8</f>
         <v>7</v>
       </c>
@@ -7191,7 +7192,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="G63" s="5">
+      <c r="G63" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7208,7 +7209,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>45</v>
       </c>
@@ -7216,7 +7217,7 @@
         <f>'Create Activities'!C9</f>
         <v>concrete, anchors</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="10">
         <f>'Create Activities'!J9</f>
         <v>8</v>
       </c>
@@ -7230,7 +7231,7 @@
         <f>'Create Activities'!$C$33</f>
         <v>concrete, mix 6000 psi</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G64" s="10">
         <f>'Create Activities'!$J$33</f>
         <v>32</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>45</v>
       </c>
@@ -7255,7 +7256,7 @@
         <f>'Create Activities'!C10</f>
         <v>steel concrete reinforcement</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="10">
         <f>'Create Activities'!J10</f>
         <v>9</v>
       </c>
@@ -7268,7 +7269,7 @@
       <c r="F65" t="s">
         <v>224</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="10" t="s">
         <v>225</v>
       </c>
       <c r="H65">
@@ -7287,7 +7288,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -7295,7 +7296,7 @@
         <f>'Create Activities'!C11</f>
         <v>steel, penstock</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="10">
         <f>'Create Activities'!J11</f>
         <v>10</v>
       </c>
@@ -7308,7 +7309,7 @@
       <c r="F66" t="s">
         <v>227</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="10" t="s">
         <v>228</v>
       </c>
       <c r="H66">
@@ -7327,7 +7328,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>45</v>
       </c>
@@ -7335,7 +7336,7 @@
         <f>'Create Activities'!C12</f>
         <v>steel, surge chamber lining</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="10">
         <f>'Create Activities'!J12</f>
         <v>11</v>
       </c>
@@ -7348,7 +7349,7 @@
       <c r="F67" t="s">
         <v>227</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="10" t="s">
         <v>228</v>
       </c>
       <c r="H67">
@@ -7364,7 +7365,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -7372,7 +7373,7 @@
         <f>'Create Activities'!$C$30</f>
         <v>copper, transformer</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="10">
         <f>'Create Activities'!$J$30</f>
         <v>29</v>
       </c>
@@ -7385,7 +7386,7 @@
       <c r="F68" t="s">
         <v>232</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="10" t="s">
         <v>234</v>
       </c>
       <c r="H68">
@@ -7401,7 +7402,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -7409,7 +7410,7 @@
         <f>'Create Activities'!$C$30</f>
         <v>copper, transformer</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C69" s="10">
         <f>'Create Activities'!$J$30</f>
         <v>29</v>
       </c>
@@ -7422,7 +7423,7 @@
       <c r="F69" t="s">
         <v>233</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="10" t="s">
         <v>235</v>
       </c>
       <c r="H69">
@@ -7438,7 +7439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>45</v>
       </c>
@@ -7446,7 +7447,7 @@
         <f>'Create Activities'!$C$13</f>
         <v>steel, transformer</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="10">
         <f>'Create Activities'!$J$13</f>
         <v>12</v>
       </c>
@@ -7459,7 +7460,7 @@
       <c r="F70" t="s">
         <v>91</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="10" t="s">
         <v>103</v>
       </c>
       <c r="H70">
@@ -7475,7 +7476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -7483,7 +7484,7 @@
         <f>'Create Activities'!$C$37</f>
         <v>polymer, transformer</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71" s="10">
         <f>'Create Activities'!$J$37</f>
         <v>36</v>
       </c>
@@ -7498,7 +7499,7 @@
         <f>'Copy Activities'!B5</f>
         <v>transformer production, high voltage use</v>
       </c>
-      <c r="G71" t="str">
+      <c r="G71" s="10" t="str">
         <f>'Copy Activities'!C5</f>
         <v>0b351f4dc4b4395c5d504e64b5c4a0a3</v>
       </c>
@@ -7518,7 +7519,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>45</v>
       </c>
@@ -7526,7 +7527,7 @@
         <f>'Create Activities'!C14</f>
         <v>steel, turbine</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="10">
         <f>'Create Activities'!J14</f>
         <v>13</v>
       </c>
@@ -7539,7 +7540,7 @@
       <c r="F72" t="s">
         <v>240</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="10" t="s">
         <v>241</v>
       </c>
       <c r="H72">
@@ -7555,7 +7556,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -7563,7 +7564,7 @@
         <f>'Create Activities'!C15</f>
         <v>steel, turbine shutoff valve</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="10">
         <f>'Create Activities'!J15</f>
         <v>14</v>
       </c>
@@ -7576,7 +7577,7 @@
       <c r="F73" t="s">
         <v>240</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="10" t="s">
         <v>241</v>
       </c>
       <c r="H73">
@@ -7592,7 +7593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>45</v>
       </c>
@@ -7600,7 +7601,7 @@
         <f>'Create Activities'!C16</f>
         <v>steel, generator</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="10">
         <f>'Create Activities'!J16</f>
         <v>15</v>
       </c>
@@ -7613,7 +7614,7 @@
       <c r="F74" t="s">
         <v>240</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" s="10" t="s">
         <v>241</v>
       </c>
       <c r="H74">
@@ -7629,14 +7630,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>45</v>
       </c>
       <c r="B75" t="s">
         <v>242</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="10" t="s">
         <v>243</v>
       </c>
       <c r="D75" s="5" t="s">
@@ -7648,7 +7649,7 @@
       <c r="F75" t="s">
         <v>79</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="10" t="s">
         <v>150</v>
       </c>
       <c r="H75">
@@ -7664,7 +7665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -7672,7 +7673,7 @@
         <f>'Create Activities'!C17</f>
         <v>water, initial reservoir fill</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="10">
         <f>'Create Activities'!J17</f>
         <v>16</v>
       </c>
@@ -7686,7 +7687,7 @@
         <f>'Copy Activities'!$B$6</f>
         <v>tap water production, underground water without treatment</v>
       </c>
-      <c r="G76" t="str">
+      <c r="G76" s="10" t="str">
         <f>'Copy Activities'!$C$6</f>
         <v>903957dbaf8147dda6c17296323caa3e</v>
       </c>
@@ -7706,7 +7707,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>45</v>
       </c>
@@ -7714,7 +7715,7 @@
         <f>'Create Activities'!C18</f>
         <v>water, annual makeup</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="10">
         <f>'Create Activities'!J18</f>
         <v>17</v>
       </c>
@@ -7728,7 +7729,7 @@
         <f>'Copy Activities'!$B$6</f>
         <v>tap water production, underground water without treatment</v>
       </c>
-      <c r="G77" t="str">
+      <c r="G77" s="10" t="str">
         <f>'Copy Activities'!$C$6</f>
         <v>903957dbaf8147dda6c17296323caa3e</v>
       </c>
@@ -7745,7 +7746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -7753,7 +7754,7 @@
         <f>'Create Activities'!C20</f>
         <v>electricity, construction</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="10">
         <f>'Create Activities'!J20</f>
         <v>19</v>
       </c>
@@ -7766,7 +7767,7 @@
       <c r="F78" t="s">
         <v>79</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="10" t="s">
         <v>150</v>
       </c>
       <c r="H78">
@@ -7782,7 +7783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -7790,7 +7791,7 @@
         <f>'Create Activities'!C21</f>
         <v>electricity, US grid mix, annual</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="10">
         <f>'Create Activities'!J21</f>
         <v>20</v>
       </c>
@@ -7803,7 +7804,7 @@
       <c r="F79" t="s">
         <v>247</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="10" t="s">
         <v>248</v>
       </c>
       <c r="H79">
@@ -7819,7 +7820,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>45</v>
       </c>
@@ -7827,7 +7828,7 @@
         <f>'Create Activities'!C22</f>
         <v>diesel, construction</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="10">
         <f>'Create Activities'!J22</f>
         <v>21</v>
       </c>
@@ -7840,7 +7841,7 @@
       <c r="F80" t="s">
         <v>251</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="10" t="s">
         <v>252</v>
       </c>
       <c r="H80">
@@ -7859,7 +7860,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>45</v>
       </c>
@@ -7867,7 +7868,7 @@
         <f>'Create Activities'!C23</f>
         <v>lubricating oil</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C81" s="10">
         <f>'Create Activities'!J23</f>
         <v>22</v>
       </c>
@@ -7880,7 +7881,7 @@
       <c r="F81" t="s">
         <v>254</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="10" t="s">
         <v>252</v>
       </c>
       <c r="H81">
@@ -7896,7 +7897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>45</v>
       </c>
@@ -7904,7 +7905,7 @@
         <f>'Create Activities'!C25</f>
         <v>transport, truck</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C82" s="10">
         <f>'Create Activities'!J25</f>
         <v>24</v>
       </c>
@@ -7917,7 +7918,7 @@
       <c r="F82" t="s">
         <v>259</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="10" t="s">
         <v>260</v>
       </c>
       <c r="H82">
@@ -7933,7 +7934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>45</v>
       </c>
@@ -7941,7 +7942,7 @@
         <f>'Create Activities'!C26</f>
         <v>transport, train</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C83" s="10">
         <f>'Create Activities'!J26</f>
         <v>25</v>
       </c>
@@ -7954,7 +7955,7 @@
       <c r="F83" t="s">
         <v>255</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="10" t="s">
         <v>256</v>
       </c>
       <c r="H83">
@@ -7973,7 +7974,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -7981,7 +7982,7 @@
         <f>'Create Activities'!C27</f>
         <v>transport, freight</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="10">
         <f>'Create Activities'!J27</f>
         <v>26</v>
       </c>
@@ -7994,7 +7995,7 @@
       <c r="F84" t="s">
         <v>261</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="10" t="s">
         <v>262</v>
       </c>
       <c r="H84">
@@ -8010,7 +8011,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -8018,7 +8019,7 @@
         <f>'Create Activities'!C28</f>
         <v>explosives, reservoir</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C85" s="10">
         <f>'Create Activities'!J28</f>
         <v>27</v>
       </c>
@@ -8031,7 +8032,7 @@
       <c r="F85" t="s">
         <v>263</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="10" t="s">
         <v>264</v>
       </c>
       <c r="H85">
@@ -8047,7 +8048,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -8055,7 +8056,7 @@
         <f>'Create Activities'!C29</f>
         <v>copper, turbine and electrical</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C86" s="10">
         <f>'Create Activities'!J29</f>
         <v>28</v>
       </c>
@@ -8068,7 +8069,7 @@
       <c r="F86" t="s">
         <v>265</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="10" t="s">
         <v>266</v>
       </c>
       <c r="H86">
@@ -8084,7 +8085,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>45</v>
       </c>
@@ -8092,7 +8093,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C87" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8105,7 +8106,7 @@
       <c r="F87" t="s">
         <v>47</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H87">
@@ -8124,7 +8125,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -8132,7 +8133,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C88" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8140,12 +8141,12 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F88" t="s">
         <v>274</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="10" t="s">
         <v>275</v>
       </c>
       <c r="H88">
@@ -8161,7 +8162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>45</v>
       </c>
@@ -8169,7 +8170,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C89" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8177,12 +8178,12 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F89" t="s">
         <v>276</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="10" t="s">
         <v>277</v>
       </c>
       <c r="H89">
@@ -8198,7 +8199,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>45</v>
       </c>
@@ -8206,7 +8207,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C90" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8214,12 +8215,12 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F90" t="s">
         <v>278</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="10" t="s">
         <v>279</v>
       </c>
       <c r="H90">
@@ -8235,7 +8236,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>45</v>
       </c>
@@ -8243,7 +8244,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C91" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8251,12 +8252,12 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F91" t="s">
         <v>271</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="10" t="s">
         <v>281</v>
       </c>
       <c r="H91">
@@ -8272,7 +8273,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -8280,7 +8281,7 @@
         <f>'Create Activities'!$C$31</f>
         <v>reservoir liner</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C92" s="10">
         <f>'Create Activities'!$J$31</f>
         <v>30</v>
       </c>
@@ -8288,12 +8289,12 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F92" t="s">
         <v>272</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="10" t="s">
         <v>282</v>
       </c>
       <c r="H92">
@@ -8309,7 +8310,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -8317,7 +8318,7 @@
         <f>'Create Activities'!C32</f>
         <v>tranmission network</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C93" s="10">
         <f>'Create Activities'!J32</f>
         <v>31</v>
       </c>
@@ -8330,7 +8331,7 @@
       <c r="F93" t="s">
         <v>269</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="10" t="s">
         <v>270</v>
       </c>
       <c r="H93">
@@ -8346,16 +8347,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C94" s="5"/>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C95" s="5"/>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D95" s="5"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C96" s="5"/>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D96" s="5"/>
     </row>
   </sheetData>
@@ -8374,15 +8372,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA05EB5AF170934C820D4EB790D7F23F" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b1015ee794e217919591e3f012a68032">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8b38413a-6683-4211-b276-15942b9b7e1d" xmlns:ns4="b818b721-7431-467d-98b7-fc0968794988" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42b2e410b11e4c78a5d1b67352e0d8f8" ns3:_="" ns4:_="">
     <xsd:import namespace="8b38413a-6683-4211-b276-15942b9b7e1d"/>
@@ -8585,6 +8574,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13499DBD-75DE-45D0-8348-E7B3B8E157DB}">
   <ds:schemaRefs>
@@ -8603,14 +8601,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C25D87A-8A1E-44A9-91B2-09FD7EEF4F75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A27E66AE-2A4D-45C9-96B7-942F327C00B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8627,4 +8617,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C25D87A-8A1E-44A9-91B2-09FD7EEF4F75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>